<commit_message>
Minha primeira versão com CustomTkinter
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -1463,7 +1463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1552,6 +1552,46 @@
           <t>30/12/2025</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>04/11/2025</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>06/11/2025</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>11/11/2025</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>13/11/2025</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>18/11/2025</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>20/11/2025</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>25/11/2025</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>27/11/2025</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -1610,6 +1650,14 @@
           <t>c</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -1623,15 +1671,75 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -1645,15 +1753,75 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1667,15 +1835,75 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
card finalizado+bt add/cancel + logica
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -993,10 +993,12 @@
           <t>Adulto A</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="n">
+        <v>46</v>
+      </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>F45+</t>
+          <t>Não definida</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
@@ -1005,14 +1007,180 @@
           <t>Masculino</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>02/11/1979</t>
-        </is>
+      <c r="M10" s="2" t="n">
+        <v>28897</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
           <t>(21) 9 9221-8787</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>julio cesar darwin</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Terça e Quinta</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>16h00</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Jefferson</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Adulto B</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>24</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Não definida</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Não Binário</t>
+        </is>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>37089</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>(19) 9 9877-1212</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>antônio de mattos</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Terça e Quinta</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>16h00</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Jefferson</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Adulto B</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>43</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Não definida</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>30294</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>(19) 9 9976-3211</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>carla camuratti</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Terça e Quinta</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>16h00</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Daniela</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Adulto A</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>G50+</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>05/09/1974</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>(21) 9 9933-2876</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
mudança sistema de filtro sem painel lateral
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -1161,10 +1161,12 @@
           <t>Adulto A</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" t="n">
+        <v>51</v>
+      </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>G50+</t>
+          <t>Não definida</t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -1173,10 +1175,8 @@
           <t>Feminino</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>05/09/1974</t>
-        </is>
+      <c r="M13" s="2" t="n">
+        <v>27158</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -2102,7 +2102,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2231,6 +2231,16 @@
           <t>27/11/2025</t>
         </is>
       </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>19/12/2025</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>24/12/2025</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -2297,6 +2307,8 @@
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -2379,6 +2391,8 @@
           <t>c</t>
         </is>
       </c>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -2461,6 +2475,8 @@
           <t>c</t>
         </is>
       </c>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -2543,6 +2559,128 @@
           <t>c</t>
         </is>
       </c>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>joão do pão</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>fernando lando</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ana cintra</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
edição das colunas da fx turmas-correções pra fazer
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1369,6 +1369,64 @@
       <c r="L16" t="inlineStr">
         <is>
           <t>13h45</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Janja da Silva</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Segunda e Quarta</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Claudia</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>46</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Não Binário</t>
+        </is>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>29110</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>(84) 9 9797-1212</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>F45+</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>11h00</t>
         </is>
       </c>
     </row>
@@ -2133,25 +2191,29 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Segunda</t>
+          <t>Segunda e Quarta</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>08h00</t>
+          <t>11h00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Adulto</t>
+          <t>Iniciação</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Ana</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr"/>
+          <t>Claudia</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
fx chamada, testes e ajustes na edição das turmas
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1421,12 +1421,244 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
+          <t>Não definida</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Lula da silva</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Segunda e Quarta</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Claudia</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Iniciação</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>73</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>19036</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>(11) 9 9877-1313</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Não definida</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Alexandre Cabeça de Pica</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Segunda e Quarta</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Claudia</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Iniciação</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>52</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>26677</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>(11) 9 9931-1533</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Não definida</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Dolores da Farmácia</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Segunda e Quarta</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>10h15</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Claudia</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>57</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>24838</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>(19) 9 9961-2344</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Não definida</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>10h15</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Jacir Novais</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Segunda e Quarta</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>10h15</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Claudia</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Nível 1</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>48</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Masculino</t>
+        </is>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>28155</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>(19) 9 9861-2346</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
           <t>F45+</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>11h00</t>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>09h30</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1673,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1929,7 +2161,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Adulto A</t>
+          <t>Adulto B</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1956,7 +2188,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Adulto B</t>
+          <t>Adulto A</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2216,6 +2448,64 @@
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Segunda e Quarta</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>10h15</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Nível 1</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Claudia</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>10h15</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Segunda e Quarta</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>09h30</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Nível 2</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Claudia</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>09h30</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2439,7 +2729,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:AT8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2576,6 +2866,106 @@
       <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>24/12/2025</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>01/12/2025</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>03/12/2025</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>05/12/2025</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>06/12/2025</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>07/12/2025</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>08/12/2025</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>10/12/2025</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>12/12/2025</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>13/12/2025</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>14/12/2025</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>15/12/2025</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>17/12/2025</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>20/12/2025</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>21/12/2025</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>22/12/2025</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>26/12/2025</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>27/12/2025</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>28/12/2025</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>31/12/2025</t>
         </is>
       </c>
     </row>
@@ -2646,6 +3036,26 @@
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -2730,6 +3140,26 @@
       </c>
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -2814,6 +3244,26 @@
       </c>
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -2898,6 +3348,26 @@
       </c>
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -2938,6 +3408,26 @@
           <t>j</t>
         </is>
       </c>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="inlineStr"/>
+      <c r="AS6" t="inlineStr"/>
+      <c r="AT6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -2978,6 +3468,26 @@
           <t>c</t>
         </is>
       </c>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
+      <c r="AR7" t="inlineStr"/>
+      <c r="AS7" t="inlineStr"/>
+      <c r="AT7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -3018,6 +3528,26 @@
           <t>c</t>
         </is>
       </c>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" t="inlineStr"/>
+      <c r="AS8" t="inlineStr"/>
+      <c r="AT8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fx chamada com bt exclusão+note
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -1653,7 +1653,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>F45+</t>
+          <t>Não definida</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -3410,12 +3410,24 @@
       </c>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
       <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="inlineStr"/>
       <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="inlineStr"/>
-      <c r="AH6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
       <c r="AI6" t="inlineStr"/>
       <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="inlineStr"/>
@@ -3470,12 +3482,24 @@
       </c>
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
       <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="inlineStr"/>
-      <c r="AH7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
       <c r="AI7" t="inlineStr"/>
       <c r="AJ7" t="inlineStr"/>
       <c r="AK7" t="inlineStr"/>
@@ -3530,12 +3554,24 @@
       </c>
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
       <c r="AD8" t="inlineStr"/>
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
       <c r="AI8" t="inlineStr"/>
       <c r="AJ8" t="inlineStr"/>
       <c r="AK8" t="inlineStr"/>

</xml_diff>

<commit_message>
ajustes de tempo real na ativação do botões ns fx chamada
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -1578,7 +1578,7 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>09h30</t>
+          <t>10h15</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AT8"/>
+  <dimension ref="A1:BC8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2966,6 +2966,51 @@
       <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>31/12/2025</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>07/01/2026</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>09/01/2026</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>14/01/2026</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>16/01/2026</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>02/01/2026</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>21/01/2026</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>23/01/2026</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>28/01/2026</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
         </is>
       </c>
     </row>
@@ -3056,6 +3101,15 @@
       <c r="AR2" t="inlineStr"/>
       <c r="AS2" t="inlineStr"/>
       <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -3160,6 +3214,15 @@
       <c r="AR3" t="inlineStr"/>
       <c r="AS3" t="inlineStr"/>
       <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="inlineStr"/>
+      <c r="AW3" t="inlineStr"/>
+      <c r="AX3" t="inlineStr"/>
+      <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="inlineStr"/>
+      <c r="BA3" t="inlineStr"/>
+      <c r="BB3" t="inlineStr"/>
+      <c r="BC3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -3264,6 +3327,15 @@
       <c r="AR4" t="inlineStr"/>
       <c r="AS4" t="inlineStr"/>
       <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="inlineStr"/>
+      <c r="AW4" t="inlineStr"/>
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -3368,6 +3440,15 @@
       <c r="AR5" t="inlineStr"/>
       <c r="AS5" t="inlineStr"/>
       <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr"/>
+      <c r="AV5" t="inlineStr"/>
+      <c r="AW5" t="inlineStr"/>
+      <c r="AX5" t="inlineStr"/>
+      <c r="AY5" t="inlineStr"/>
+      <c r="AZ5" t="inlineStr"/>
+      <c r="BA5" t="inlineStr"/>
+      <c r="BB5" t="inlineStr"/>
+      <c r="BC5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -3440,6 +3521,51 @@
       <c r="AR6" t="inlineStr"/>
       <c r="AS6" t="inlineStr"/>
       <c r="AT6" t="inlineStr"/>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AY6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AZ6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="BA6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="BB6" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="BC6" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -3512,6 +3638,51 @@
       <c r="AR7" t="inlineStr"/>
       <c r="AS7" t="inlineStr"/>
       <c r="AT7" t="inlineStr"/>
+      <c r="AU7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AV7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AW7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AX7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AY7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AZ7" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="BA7" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="BB7" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="BC7" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -3584,6 +3755,51 @@
       <c r="AR8" t="inlineStr"/>
       <c r="AS8" t="inlineStr"/>
       <c r="AT8" t="inlineStr"/>
+      <c r="AU8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AV8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AW8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AX8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AY8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="AZ8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="BA8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="BB8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="BC8" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
limpar e desfazer chamada,ok
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Turmas" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Categorias" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Registros" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Justificativas" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3521,51 +3522,19 @@
       <c r="AR6" t="inlineStr"/>
       <c r="AS6" t="inlineStr"/>
       <c r="AT6" t="inlineStr"/>
-      <c r="AU6" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="AV6" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="AW6" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="AX6" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
+      <c r="AU6" t="inlineStr"/>
+      <c r="AV6" t="inlineStr"/>
+      <c r="AW6" t="inlineStr"/>
+      <c r="AX6" t="inlineStr"/>
       <c r="AY6" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
-      <c r="AZ6" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="BA6" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="BB6" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="BC6" t="inlineStr">
-        <is>
-          <t>j</t>
-        </is>
-      </c>
+      <c r="AZ6" t="inlineStr"/>
+      <c r="BA6" t="inlineStr"/>
+      <c r="BB6" t="inlineStr"/>
+      <c r="BC6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -3638,51 +3607,19 @@
       <c r="AR7" t="inlineStr"/>
       <c r="AS7" t="inlineStr"/>
       <c r="AT7" t="inlineStr"/>
-      <c r="AU7" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="AV7" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="AW7" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="AX7" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
+      <c r="AU7" t="inlineStr"/>
+      <c r="AV7" t="inlineStr"/>
+      <c r="AW7" t="inlineStr"/>
+      <c r="AX7" t="inlineStr"/>
       <c r="AY7" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
-      <c r="AZ7" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="BA7" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
-      <c r="BB7" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
-      <c r="BC7" t="inlineStr">
-        <is>
-          <t>j</t>
-        </is>
-      </c>
+      <c r="AZ7" t="inlineStr"/>
+      <c r="BA7" t="inlineStr"/>
+      <c r="BB7" t="inlineStr"/>
+      <c r="BC7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -3755,49 +3692,87 @@
       <c r="AR8" t="inlineStr"/>
       <c r="AS8" t="inlineStr"/>
       <c r="AT8" t="inlineStr"/>
-      <c r="AU8" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="AV8" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="AW8" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="AX8" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
+      <c r="AU8" t="inlineStr"/>
+      <c r="AV8" t="inlineStr"/>
+      <c r="AW8" t="inlineStr"/>
+      <c r="AX8" t="inlineStr"/>
       <c r="AY8" t="inlineStr">
         <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="AZ8" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="BA8" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="BB8" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="BC8" t="inlineStr">
-        <is>
-          <t>c</t>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="AZ8" t="inlineStr"/>
+      <c r="BA8" t="inlineStr"/>
+      <c r="BB8" t="inlineStr"/>
+      <c r="BC8" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Motivo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ana cintra</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>23/01/2026</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>médico</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ana cintra</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>frio</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
- falta verificação lógica das exclusões
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Categorias" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Registros" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Justificativas" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Exclusões" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -433,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1376,7 +1377,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Janja da Silva</t>
+          <t>Lula da silva</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1401,23 +1402,23 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Iniciação</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Não Binário</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="I17" s="2" t="n">
-        <v>29110</v>
+        <v>19036</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>(84) 9 9797-1212</t>
+          <t>(11) 9 9877-1313</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1434,7 +1435,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Lula da silva</t>
+          <t>Alexandre Cabeça de Pica</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1463,7 +1464,7 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1471,11 +1472,11 @@
         </is>
       </c>
       <c r="I18" s="2" t="n">
-        <v>19036</v>
+        <v>26677</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>(11) 9 9877-1313</t>
+          <t>(11) 9 9931-1533</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1492,7 +1493,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Alexandre Cabeça de Pica</t>
+          <t>Dolores da Farmácia</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1507,7 +1508,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>11h00</t>
+          <t>10h15</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1517,23 +1518,23 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Iniciação</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="I19" s="2" t="n">
-        <v>26677</v>
+        <v>24838</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>(11) 9 9931-1533</t>
+          <t>(19) 9 9961-2344</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1543,14 +1544,14 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>11h00</t>
+          <t>10h15</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Dolores da Farmácia</t>
+          <t>Jacir Novais</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1575,23 +1576,23 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Nível 1</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="I20" s="2" t="n">
-        <v>24838</v>
+        <v>28155</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>(19) 9 9961-2344</t>
+          <t>(19) 9 9861-2346</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1600,64 +1601,6 @@
         </is>
       </c>
       <c r="L20" t="inlineStr">
-        <is>
-          <t>10h15</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Jacir Novais</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Segunda e Quarta</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>10h15</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Claudia</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Nível 1</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
-        <v>48</v>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Masculino</t>
-        </is>
-      </c>
-      <c r="I21" s="2" t="n">
-        <v>28155</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>(19) 9 9861-2346</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Não definida</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
         <is>
           <t>10h15</t>
         </is>
@@ -2730,7 +2673,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BC8"/>
+  <dimension ref="A1:BY11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3012,6 +2955,116 @@
       <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>30/01/2026</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>01/01/2026</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>04/01/2026</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>05/01/2026</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>06/01/2026</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>08/01/2026</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>10/01/2026</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>11/01/2026</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>12/01/2026</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>13/01/2026</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>15/01/2026</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>17/01/2026</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>18/01/2026</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>20/01/2026</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>22/01/2026</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>24/01/2026</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>25/01/2026</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>26/01/2026</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>27/01/2026</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>29/01/2026</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>31/01/2026</t>
         </is>
       </c>
     </row>
@@ -3111,6 +3164,28 @@
       <c r="BA2" t="inlineStr"/>
       <c r="BB2" t="inlineStr"/>
       <c r="BC2" t="inlineStr"/>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="inlineStr"/>
+      <c r="BI2" t="inlineStr"/>
+      <c r="BJ2" t="inlineStr"/>
+      <c r="BK2" t="inlineStr"/>
+      <c r="BL2" t="inlineStr"/>
+      <c r="BM2" t="inlineStr"/>
+      <c r="BN2" t="inlineStr"/>
+      <c r="BO2" t="inlineStr"/>
+      <c r="BP2" t="inlineStr"/>
+      <c r="BQ2" t="inlineStr"/>
+      <c r="BR2" t="inlineStr"/>
+      <c r="BS2" t="inlineStr"/>
+      <c r="BT2" t="inlineStr"/>
+      <c r="BU2" t="inlineStr"/>
+      <c r="BV2" t="inlineStr"/>
+      <c r="BW2" t="inlineStr"/>
+      <c r="BX2" t="inlineStr"/>
+      <c r="BY2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -3224,6 +3299,28 @@
       <c r="BA3" t="inlineStr"/>
       <c r="BB3" t="inlineStr"/>
       <c r="BC3" t="inlineStr"/>
+      <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="inlineStr"/>
+      <c r="BF3" t="inlineStr"/>
+      <c r="BG3" t="inlineStr"/>
+      <c r="BH3" t="inlineStr"/>
+      <c r="BI3" t="inlineStr"/>
+      <c r="BJ3" t="inlineStr"/>
+      <c r="BK3" t="inlineStr"/>
+      <c r="BL3" t="inlineStr"/>
+      <c r="BM3" t="inlineStr"/>
+      <c r="BN3" t="inlineStr"/>
+      <c r="BO3" t="inlineStr"/>
+      <c r="BP3" t="inlineStr"/>
+      <c r="BQ3" t="inlineStr"/>
+      <c r="BR3" t="inlineStr"/>
+      <c r="BS3" t="inlineStr"/>
+      <c r="BT3" t="inlineStr"/>
+      <c r="BU3" t="inlineStr"/>
+      <c r="BV3" t="inlineStr"/>
+      <c r="BW3" t="inlineStr"/>
+      <c r="BX3" t="inlineStr"/>
+      <c r="BY3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -3337,6 +3434,28 @@
       <c r="BA4" t="inlineStr"/>
       <c r="BB4" t="inlineStr"/>
       <c r="BC4" t="inlineStr"/>
+      <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr"/>
+      <c r="BF4" t="inlineStr"/>
+      <c r="BG4" t="inlineStr"/>
+      <c r="BH4" t="inlineStr"/>
+      <c r="BI4" t="inlineStr"/>
+      <c r="BJ4" t="inlineStr"/>
+      <c r="BK4" t="inlineStr"/>
+      <c r="BL4" t="inlineStr"/>
+      <c r="BM4" t="inlineStr"/>
+      <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr"/>
+      <c r="BP4" t="inlineStr"/>
+      <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="inlineStr"/>
+      <c r="BS4" t="inlineStr"/>
+      <c r="BT4" t="inlineStr"/>
+      <c r="BU4" t="inlineStr"/>
+      <c r="BV4" t="inlineStr"/>
+      <c r="BW4" t="inlineStr"/>
+      <c r="BX4" t="inlineStr"/>
+      <c r="BY4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -3450,6 +3569,28 @@
       <c r="BA5" t="inlineStr"/>
       <c r="BB5" t="inlineStr"/>
       <c r="BC5" t="inlineStr"/>
+      <c r="BD5" t="inlineStr"/>
+      <c r="BE5" t="inlineStr"/>
+      <c r="BF5" t="inlineStr"/>
+      <c r="BG5" t="inlineStr"/>
+      <c r="BH5" t="inlineStr"/>
+      <c r="BI5" t="inlineStr"/>
+      <c r="BJ5" t="inlineStr"/>
+      <c r="BK5" t="inlineStr"/>
+      <c r="BL5" t="inlineStr"/>
+      <c r="BM5" t="inlineStr"/>
+      <c r="BN5" t="inlineStr"/>
+      <c r="BO5" t="inlineStr"/>
+      <c r="BP5" t="inlineStr"/>
+      <c r="BQ5" t="inlineStr"/>
+      <c r="BR5" t="inlineStr"/>
+      <c r="BS5" t="inlineStr"/>
+      <c r="BT5" t="inlineStr"/>
+      <c r="BU5" t="inlineStr"/>
+      <c r="BV5" t="inlineStr"/>
+      <c r="BW5" t="inlineStr"/>
+      <c r="BX5" t="inlineStr"/>
+      <c r="BY5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -3535,6 +3676,28 @@
       <c r="BA6" t="inlineStr"/>
       <c r="BB6" t="inlineStr"/>
       <c r="BC6" t="inlineStr"/>
+      <c r="BD6" t="inlineStr"/>
+      <c r="BE6" t="inlineStr"/>
+      <c r="BF6" t="inlineStr"/>
+      <c r="BG6" t="inlineStr"/>
+      <c r="BH6" t="inlineStr"/>
+      <c r="BI6" t="inlineStr"/>
+      <c r="BJ6" t="inlineStr"/>
+      <c r="BK6" t="inlineStr"/>
+      <c r="BL6" t="inlineStr"/>
+      <c r="BM6" t="inlineStr"/>
+      <c r="BN6" t="inlineStr"/>
+      <c r="BO6" t="inlineStr"/>
+      <c r="BP6" t="inlineStr"/>
+      <c r="BQ6" t="inlineStr"/>
+      <c r="BR6" t="inlineStr"/>
+      <c r="BS6" t="inlineStr"/>
+      <c r="BT6" t="inlineStr"/>
+      <c r="BU6" t="inlineStr"/>
+      <c r="BV6" t="inlineStr"/>
+      <c r="BW6" t="inlineStr"/>
+      <c r="BX6" t="inlineStr"/>
+      <c r="BY6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -3620,6 +3783,28 @@
       <c r="BA7" t="inlineStr"/>
       <c r="BB7" t="inlineStr"/>
       <c r="BC7" t="inlineStr"/>
+      <c r="BD7" t="inlineStr"/>
+      <c r="BE7" t="inlineStr"/>
+      <c r="BF7" t="inlineStr"/>
+      <c r="BG7" t="inlineStr"/>
+      <c r="BH7" t="inlineStr"/>
+      <c r="BI7" t="inlineStr"/>
+      <c r="BJ7" t="inlineStr"/>
+      <c r="BK7" t="inlineStr"/>
+      <c r="BL7" t="inlineStr"/>
+      <c r="BM7" t="inlineStr"/>
+      <c r="BN7" t="inlineStr"/>
+      <c r="BO7" t="inlineStr"/>
+      <c r="BP7" t="inlineStr"/>
+      <c r="BQ7" t="inlineStr"/>
+      <c r="BR7" t="inlineStr"/>
+      <c r="BS7" t="inlineStr"/>
+      <c r="BT7" t="inlineStr"/>
+      <c r="BU7" t="inlineStr"/>
+      <c r="BV7" t="inlineStr"/>
+      <c r="BW7" t="inlineStr"/>
+      <c r="BX7" t="inlineStr"/>
+      <c r="BY7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -3705,6 +3890,285 @@
       <c r="BA8" t="inlineStr"/>
       <c r="BB8" t="inlineStr"/>
       <c r="BC8" t="inlineStr"/>
+      <c r="BD8" t="inlineStr"/>
+      <c r="BE8" t="inlineStr"/>
+      <c r="BF8" t="inlineStr"/>
+      <c r="BG8" t="inlineStr"/>
+      <c r="BH8" t="inlineStr"/>
+      <c r="BI8" t="inlineStr"/>
+      <c r="BJ8" t="inlineStr"/>
+      <c r="BK8" t="inlineStr"/>
+      <c r="BL8" t="inlineStr"/>
+      <c r="BM8" t="inlineStr"/>
+      <c r="BN8" t="inlineStr"/>
+      <c r="BO8" t="inlineStr"/>
+      <c r="BP8" t="inlineStr"/>
+      <c r="BQ8" t="inlineStr"/>
+      <c r="BR8" t="inlineStr"/>
+      <c r="BS8" t="inlineStr"/>
+      <c r="BT8" t="inlineStr"/>
+      <c r="BU8" t="inlineStr"/>
+      <c r="BV8" t="inlineStr"/>
+      <c r="BW8" t="inlineStr"/>
+      <c r="BX8" t="inlineStr"/>
+      <c r="BY8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Janja da Silva</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
+      <c r="AR9" t="inlineStr"/>
+      <c r="AS9" t="inlineStr"/>
+      <c r="AT9" t="inlineStr"/>
+      <c r="AU9" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="AV9" t="inlineStr"/>
+      <c r="AW9" t="inlineStr"/>
+      <c r="AX9" t="inlineStr"/>
+      <c r="AY9" t="inlineStr"/>
+      <c r="AZ9" t="inlineStr"/>
+      <c r="BA9" t="inlineStr"/>
+      <c r="BB9" t="inlineStr"/>
+      <c r="BC9" t="inlineStr"/>
+      <c r="BD9" t="inlineStr"/>
+      <c r="BE9" t="inlineStr"/>
+      <c r="BF9" t="inlineStr"/>
+      <c r="BG9" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="BH9" t="inlineStr"/>
+      <c r="BI9" t="inlineStr"/>
+      <c r="BJ9" t="inlineStr"/>
+      <c r="BK9" t="inlineStr"/>
+      <c r="BL9" t="inlineStr"/>
+      <c r="BM9" t="inlineStr"/>
+      <c r="BN9" t="inlineStr"/>
+      <c r="BO9" t="inlineStr"/>
+      <c r="BP9" t="inlineStr"/>
+      <c r="BQ9" t="inlineStr"/>
+      <c r="BR9" t="inlineStr"/>
+      <c r="BS9" t="inlineStr"/>
+      <c r="BT9" t="inlineStr"/>
+      <c r="BU9" t="inlineStr"/>
+      <c r="BV9" t="inlineStr"/>
+      <c r="BW9" t="inlineStr"/>
+      <c r="BX9" t="inlineStr"/>
+      <c r="BY9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Lula da silva</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
+      <c r="AR10" t="inlineStr"/>
+      <c r="AS10" t="inlineStr"/>
+      <c r="AT10" t="inlineStr"/>
+      <c r="AU10" t="inlineStr"/>
+      <c r="AV10" t="inlineStr"/>
+      <c r="AW10" t="inlineStr"/>
+      <c r="AX10" t="inlineStr"/>
+      <c r="AY10" t="inlineStr"/>
+      <c r="AZ10" t="inlineStr"/>
+      <c r="BA10" t="inlineStr"/>
+      <c r="BB10" t="inlineStr"/>
+      <c r="BC10" t="inlineStr"/>
+      <c r="BD10" t="inlineStr"/>
+      <c r="BE10" t="inlineStr"/>
+      <c r="BF10" t="inlineStr"/>
+      <c r="BG10" t="inlineStr"/>
+      <c r="BH10" t="inlineStr"/>
+      <c r="BI10" t="inlineStr"/>
+      <c r="BJ10" t="inlineStr"/>
+      <c r="BK10" t="inlineStr"/>
+      <c r="BL10" t="inlineStr"/>
+      <c r="BM10" t="inlineStr"/>
+      <c r="BN10" t="inlineStr"/>
+      <c r="BO10" t="inlineStr"/>
+      <c r="BP10" t="inlineStr"/>
+      <c r="BQ10" t="inlineStr"/>
+      <c r="BR10" t="inlineStr"/>
+      <c r="BS10" t="inlineStr"/>
+      <c r="BT10" t="inlineStr"/>
+      <c r="BU10" t="inlineStr"/>
+      <c r="BV10" t="inlineStr"/>
+      <c r="BW10" t="inlineStr"/>
+      <c r="BX10" t="inlineStr"/>
+      <c r="BY10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Alexandre Cabeça de Pica</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
+      <c r="AB11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
+      <c r="AR11" t="inlineStr"/>
+      <c r="AS11" t="inlineStr"/>
+      <c r="AT11" t="inlineStr"/>
+      <c r="AU11" t="inlineStr"/>
+      <c r="AV11" t="inlineStr"/>
+      <c r="AW11" t="inlineStr"/>
+      <c r="AX11" t="inlineStr"/>
+      <c r="AY11" t="inlineStr"/>
+      <c r="AZ11" t="inlineStr"/>
+      <c r="BA11" t="inlineStr"/>
+      <c r="BB11" t="inlineStr"/>
+      <c r="BC11" t="inlineStr"/>
+      <c r="BD11" t="inlineStr"/>
+      <c r="BE11" t="inlineStr"/>
+      <c r="BF11" t="inlineStr"/>
+      <c r="BG11" t="inlineStr"/>
+      <c r="BH11" t="inlineStr"/>
+      <c r="BI11" t="inlineStr"/>
+      <c r="BJ11" t="inlineStr"/>
+      <c r="BK11" t="inlineStr"/>
+      <c r="BL11" t="inlineStr"/>
+      <c r="BM11" t="inlineStr"/>
+      <c r="BN11" t="inlineStr"/>
+      <c r="BO11" t="inlineStr"/>
+      <c r="BP11" t="inlineStr"/>
+      <c r="BQ11" t="inlineStr"/>
+      <c r="BR11" t="inlineStr"/>
+      <c r="BS11" t="inlineStr"/>
+      <c r="BT11" t="inlineStr"/>
+      <c r="BU11" t="inlineStr"/>
+      <c r="BV11" t="inlineStr"/>
+      <c r="BW11" t="inlineStr"/>
+      <c r="BX11" t="inlineStr"/>
+      <c r="BY11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3717,7 +4181,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3776,6 +4240,187 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Janja da Silva</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>05/01/2026</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>frio</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Janja da Silva</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>07/01/2026</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>chuva</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Turma</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Horário</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Data Exclusão</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ParQ</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Nível</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Idade</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Gênero</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Data de Nascimento</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Whatsapp</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Categoria</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Horario_Formatado</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Janja da Silva</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Segunda e Quarta</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Claudia</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>46025.10740575946</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>46</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Não Binário</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>29110</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>(84) 9 9797-1212</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Não definida</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>11h00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fx relatório de chamada - acertos, frames, ano, mes
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -4382,7 +4382,7 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>46026.69448247348</v>
+        <v>46027.41603372576</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Adulto A</t>
+          <t>Adulto B</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -4403,7 +4403,7 @@
         </is>
       </c>
       <c r="J2" s="2" t="n">
-        <v>40129</v>
+        <v>40158</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
card ver na fx relatorio corrigido
</commit_message>
<xml_diff>
--- a/chamadaBelaVista.xlsx
+++ b/chamadaBelaVista.xlsx
@@ -3964,11 +3964,7 @@
       <c r="AR9" t="inlineStr"/>
       <c r="AS9" t="inlineStr"/>
       <c r="AT9" t="inlineStr"/>
-      <c r="AU9" t="inlineStr">
-        <is>
-          <t>j</t>
-        </is>
-      </c>
+      <c r="AU9" t="inlineStr"/>
       <c r="AV9" t="inlineStr"/>
       <c r="AW9" t="inlineStr"/>
       <c r="AX9" t="inlineStr"/>
@@ -4067,7 +4063,11 @@
       <c r="BD10" t="inlineStr"/>
       <c r="BE10" t="inlineStr"/>
       <c r="BF10" t="inlineStr"/>
-      <c r="BG10" t="inlineStr"/>
+      <c r="BG10" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
       <c r="BH10" t="inlineStr"/>
       <c r="BI10" t="inlineStr"/>
       <c r="BJ10" t="inlineStr"/>
@@ -4150,7 +4150,11 @@
       <c r="BD11" t="inlineStr"/>
       <c r="BE11" t="inlineStr"/>
       <c r="BF11" t="inlineStr"/>
-      <c r="BG11" t="inlineStr"/>
+      <c r="BG11" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
       <c r="BH11" t="inlineStr"/>
       <c r="BI11" t="inlineStr"/>
       <c r="BJ11" t="inlineStr"/>
@@ -4382,7 +4386,7 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>46027.41603372576</v>
+        <v>46027.41603372685</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>

</xml_diff>